<commit_message>
handle no header dfs outside of Excel tables & fix aggsum/maxrows tests
</commit_message>
<xml_diff>
--- a/tests/reports/df_filter_frame.xlsx
+++ b/tests/reports/df_filter_frame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\tests\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B8A3E9-E4A7-C948-BA04-B50023858348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF7BF80-1423-4C75-B489-BF23AFE26D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3960" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>&lt;frame&gt;</t>
   </si>
@@ -61,16 +61,16 @@
     <t>Static Text</t>
   </si>
   <si>
-    <t>{{ df2 | maxrows(2)}}</t>
-  </si>
-  <si>
-    <t>{{ df2 | noheader | maxrows(2) }}</t>
-  </si>
-  <si>
     <t>{{ mystring }}</t>
   </si>
   <si>
     <t>stringtest</t>
+  </si>
+  <si>
+    <t>{{ df2 | maxrows(2, Other, 0)}}</t>
+  </si>
+  <si>
+    <t>{{ df2 | noheader | maxrows(2, Other, 0) }}</t>
   </si>
 </sst>
 </file>
@@ -438,62 +438,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CDD2CB-3C5D-A643-8BB3-87BAF428157A}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.8125" style="2"/>
+    <col min="2" max="16384" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -506,22 +497,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E17503-0AF3-7F4E-8C35-34AC82F719A2}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.8125" style="2"/>
+    <col min="2" max="16384" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -536,7 +525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" s="4">
         <v>0</v>
       </c>
@@ -553,9 +542,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>1</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
@@ -570,26 +559,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A7" s="4">
         <v>0</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>4</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>1</v>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
@@ -604,7 +593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Filter fixes and additions (Part II of #1626) (#1632)
* filter fixes

* fix excel tables without headers

* handle no header dfs outside of Excel tables & fix aggsum/maxrows tests

* added "body" filter for dataframes

* docs [skip ci]
</commit_message>
<xml_diff>
--- a/tests/reports/df_filter_frame.xlsx
+++ b/tests/reports/df_filter_frame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\tests\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B8A3E9-E4A7-C948-BA04-B50023858348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF7BF80-1423-4C75-B489-BF23AFE26D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3960" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>&lt;frame&gt;</t>
   </si>
@@ -61,16 +61,16 @@
     <t>Static Text</t>
   </si>
   <si>
-    <t>{{ df2 | maxrows(2)}}</t>
-  </si>
-  <si>
-    <t>{{ df2 | noheader | maxrows(2) }}</t>
-  </si>
-  <si>
     <t>{{ mystring }}</t>
   </si>
   <si>
     <t>stringtest</t>
+  </si>
+  <si>
+    <t>{{ df2 | maxrows(2, Other, 0)}}</t>
+  </si>
+  <si>
+    <t>{{ df2 | noheader | maxrows(2, Other, 0) }}</t>
   </si>
 </sst>
 </file>
@@ -438,62 +438,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CDD2CB-3C5D-A643-8BB3-87BAF428157A}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.8125" style="2"/>
+    <col min="2" max="16384" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -506,22 +497,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E17503-0AF3-7F4E-8C35-34AC82F719A2}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.8125" style="2"/>
+    <col min="2" max="16384" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -536,7 +525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" s="4">
         <v>0</v>
       </c>
@@ -553,9 +542,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>1</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
@@ -570,26 +559,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A7" s="4">
         <v>0</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>4</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>1</v>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
@@ -604,7 +593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Adds basic support for Notes and Print_Area / pro.reports: Frame refactor & preserve print_area (#1641)
* added range.comment

* read frame markers from Notes

* macOS fix

* renamed comments to notes

* (test) fixes

* added test

* docs

* simplify

* docs

* added note.delete()

* delete <frame> notes after rendering a template

* added page_setup.print_area

* page_setup windows fixes

* preserve print_area with reports
</commit_message>
<xml_diff>
--- a/tests/reports/df_filter_frame.xlsx
+++ b/tests/reports/df_filter_frame.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\tests\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF7BF80-1423-4C75-B489-BF23AFE26D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC02443-3767-4106-B0BB-E9A764762BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="expected" sheetId="9" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,11 +34,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Felix Zumstein</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{DEAED013-E257-4349-A3AF-80243C2ABD58}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>&lt;frame&gt;</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
-  <si>
-    <t>&lt;frame&gt;</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>a</t>
   </si>
@@ -77,13 +98,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -437,10 +465,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CDD2CB-3C5D-A643-8BB3-87BAF428157A}">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CDD2CB-3C5D-A643-8BB3-87BAF428157A}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
@@ -450,46 +480,42 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -507,22 +533,22 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.5">
@@ -530,7 +556,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="4">
         <v>4</v>
@@ -544,10 +570,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="4">
         <v>23</v>
@@ -564,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="4">
         <v>4</v>
@@ -578,10 +604,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4">
         <v>23</v>
@@ -595,7 +621,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added datetime filter and fixed string arguments in filters (breaking change)
</commit_message>
<xml_diff>
--- a/tests/reports/df_filter_frame.xlsx
+++ b/tests/reports/df_filter_frame.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\tests\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC02443-3767-4106-B0BB-E9A764762BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328CC0EA-9A46-1643-A145-C7E88CDFE96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
+    <workbookView xWindow="960" yWindow="500" windowWidth="23240" windowHeight="14000" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="expected" sheetId="9" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +48,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>&lt;frame&gt;</t>
         </r>
@@ -88,10 +88,10 @@
     <t>stringtest</t>
   </si>
   <si>
-    <t>{{ df2 | maxrows(2, Other, 0)}}</t>
-  </si>
-  <si>
-    <t>{{ df2 | noheader | maxrows(2, Other, 0) }}</t>
+    <t>{{ df2 | maxrows(2, "Other", 0)}}</t>
+  </si>
+  <si>
+    <t>{{ df2 | noheader | maxrows(2, "Other", 0) }}</t>
   </si>
 </sst>
 </file>
@@ -111,7 +111,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -469,21 +469,21 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8125" style="2"/>
-    <col min="2" max="16384" width="10.8125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -492,14 +492,14 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -508,7 +508,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -525,18 +525,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8125" style="2"/>
-    <col min="2" max="16384" width="10.8125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -551,7 +551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>0</v>
       </c>
@@ -568,7 +568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -585,7 +585,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>0</v>
       </c>
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -619,7 +619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Reports: datetime and arithmetic filters / breaking change: filter string args must be Excel strings (#1674)
* added datetime filter
* fixed string arguments in filters (breaking change)
* added multiply/divide/subtract/add df filters
</commit_message>
<xml_diff>
--- a/tests/reports/df_filter_frame.xlsx
+++ b/tests/reports/df_filter_frame.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\tests\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC02443-3767-4106-B0BB-E9A764762BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328CC0EA-9A46-1643-A145-C7E88CDFE96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
+    <workbookView xWindow="960" yWindow="500" windowWidth="23240" windowHeight="14000" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="expected" sheetId="9" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +48,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>&lt;frame&gt;</t>
         </r>
@@ -88,10 +88,10 @@
     <t>stringtest</t>
   </si>
   <si>
-    <t>{{ df2 | maxrows(2, Other, 0)}}</t>
-  </si>
-  <si>
-    <t>{{ df2 | noheader | maxrows(2, Other, 0) }}</t>
+    <t>{{ df2 | maxrows(2, "Other", 0)}}</t>
+  </si>
+  <si>
+    <t>{{ df2 | noheader | maxrows(2, "Other", 0) }}</t>
   </si>
 </sst>
 </file>
@@ -111,7 +111,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -469,21 +469,21 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8125" style="2"/>
-    <col min="2" max="16384" width="10.8125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -492,14 +492,14 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -508,7 +508,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -525,18 +525,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8125" style="2"/>
-    <col min="2" max="16384" width="10.8125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -551,7 +551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>0</v>
       </c>
@@ -568,7 +568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -585,7 +585,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>0</v>
       </c>
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -619,7 +619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
fixing tests, refactor arithmetic filters to abbreviated version and cleaned up docs
</commit_message>
<xml_diff>
--- a/tests/reports/df_filter_frame.xlsx
+++ b/tests/reports/df_filter_frame.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328CC0EA-9A46-1643-A145-C7E88CDFE96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE11314-24C7-0242-B1B4-DF4F0A4F8B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="500" windowWidth="23240" windowHeight="14000" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
+    <workbookView xWindow="960" yWindow="500" windowWidth="23240" windowHeight="14000" activeTab="1" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>a</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>{{ df2 | noheader | maxrows(2, "Other", 0) }}</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CDD2CB-3C5D-A643-8BB3-87BAF428157A}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -523,7 +526,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E17503-0AF3-7F4E-8C35-34AC82F719A2}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -537,7 +542,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -572,9 +579,7 @@
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="4">
         <v>23</v>
       </c>
@@ -606,9 +611,7 @@
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="4">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
fix 'header' filter in frames
</commit_message>
<xml_diff>
--- a/tests/reports/df_filter_frame.xlsx
+++ b/tests/reports/df_filter_frame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\tests\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE11314-24C7-0242-B1B4-DF4F0A4F8B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB9D615-AF76-4CF7-9CAC-5503DC9D275A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="500" windowWidth="23240" windowHeight="14000" activeTab="1" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>a</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>{{ df2 | header }}</t>
   </si>
 </sst>
 </file>
@@ -469,24 +472,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CDD2CB-3C5D-A643-8BB3-87BAF428157A}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.8125" style="2"/>
+    <col min="2" max="16384" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -495,24 +498,29 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -524,24 +532,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E17503-0AF3-7F4E-8C35-34AC82F719A2}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.8125" style="2"/>
+    <col min="2" max="16384" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -558,7 +566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" s="4">
         <v>0</v>
       </c>
@@ -575,7 +583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -590,40 +598,57 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A8" s="4">
         <v>0</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C8" s="4">
         <v>4</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D8" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E8" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4">
         <v>23</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9" s="4">
         <v>22</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E9" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added vmerge DataFrame filter for pro.reports
</commit_message>
<xml_diff>
--- a/tests/reports/df_filter_frame.xlsx
+++ b/tests/reports/df_filter_frame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\tests\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB9D615-AF76-4CF7-9CAC-5503DC9D275A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CF0826-02A1-444E-B74D-EF11DD633095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
+    <workbookView xWindow="1560" yWindow="-16220" windowWidth="23240" windowHeight="14000" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>a</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>{{ df2 | header }}</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>{{ df3 | vmerge(0, 1) }}</t>
   </si>
 </sst>
 </file>
@@ -115,12 +124,12 @@
     <font>
       <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,11 +148,69 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -152,12 +219,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,24 +552,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CDD2CB-3C5D-A643-8BB3-87BAF428157A}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8125" style="2"/>
-    <col min="2" max="16384" width="10.8125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -498,19 +578,19 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -519,10 +599,20 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -532,24 +622,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E17503-0AF3-7F4E-8C35-34AC82F719A2}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8125" style="2"/>
-    <col min="2" max="16384" width="10.8125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -566,7 +656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>0</v>
       </c>
@@ -583,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -598,7 +688,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -615,7 +705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>0</v>
       </c>
@@ -632,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -647,12 +737,75 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="9"/>
+      <c r="B17" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A20:A21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Formatters for Range.options() and as filters for xlwings.reports (#2051)
* added "formatter" callback for both basic API and xlwings Reports

* docs

* unit tests
</commit_message>
<xml_diff>
--- a/tests/reports/df_filter_frame.xlsx
+++ b/tests/reports/df_filter_frame.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CF0826-02A1-444E-B74D-EF11DD633095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5C9157-8C10-2443-85CC-24250F6055AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="-16220" windowWidth="23240" windowHeight="14000" xr2:uid="{B71C96D3-0AD6-FC4B-A0E6-7709A49D647A}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
   <si>
     <t>a</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>{{ df3 | vmerge(0, 1) }}</t>
+  </si>
+  <si>
+    <t>{{ df3 | formatter("table") }}</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +157,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -219,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -229,6 +244,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -552,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CDD2CB-3C5D-A643-8BB3-87BAF428157A}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,6 +631,11 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -622,10 +644,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E17503-0AF3-7F4E-8C35-34AC82F719A2}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,7 +773,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -759,26 +781,26 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="8"/>
+      <c r="A16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="10"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -786,17 +808,89 @@
       <c r="A19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="9"/>
+      <c r="B19" s="11"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="9"/>
+      <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>